<commit_message>
RegTools and LAG Working
</commit_message>
<xml_diff>
--- a/mbs-EP-v.1.0.1/Excel Files/flyball_governor_damper_spring.xlsx
+++ b/mbs-EP-v.1.0.1/Excel Files/flyball_governor_damper_spring.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago_Serralha\Desktop\Thesis-Project\mbs-EP-v.1.0.1\Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43015F1E-F3A6-4E2B-A434-190986CA2A4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{427D7388-8B9D-456F-BFB7-0B41C7DC58B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SimParam" sheetId="4" r:id="rId1"/>
@@ -1308,6 +1308,42 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1347,21 +1383,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1419,46 +1440,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1470,15 +1479,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1494,6 +1494,36 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1519,36 +1549,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1984,7 +1984,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE954C49-6E73-4D49-8054-42AF7A10140C}">
   <dimension ref="B2:Q39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -2004,44 +2004,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B2" s="109" t="s">
+      <c r="B2" s="75" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="110"/>
-      <c r="D2" s="110"/>
-      <c r="E2" s="111"/>
-      <c r="J2" s="108" t="s">
+      <c r="C2" s="76"/>
+      <c r="D2" s="76"/>
+      <c r="E2" s="77"/>
+      <c r="J2" s="71" t="s">
         <v>157</v>
       </c>
-      <c r="K2" s="108"/>
-      <c r="L2" s="108"/>
-      <c r="M2" s="108"/>
-      <c r="N2" s="108"/>
-      <c r="O2" s="108"/>
-      <c r="P2" s="108"/>
-      <c r="Q2" s="108"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="71"/>
+      <c r="M2" s="71"/>
+      <c r="N2" s="71"/>
+      <c r="O2" s="71"/>
+      <c r="P2" s="71"/>
+      <c r="Q2" s="71"/>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="86"/>
+      <c r="C3" s="74"/>
       <c r="D3" s="51">
         <v>10</v>
       </c>
       <c r="E3" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="J3" s="87" t="s">
+      <c r="J3" s="78" t="s">
         <v>106</v>
       </c>
-      <c r="K3" s="88"/>
-      <c r="L3" s="112"/>
-      <c r="M3" s="87" t="s">
+      <c r="K3" s="79"/>
+      <c r="L3" s="80"/>
+      <c r="M3" s="78" t="s">
         <v>132</v>
       </c>
-      <c r="N3" s="88"/>
-      <c r="O3" s="80"/>
+      <c r="N3" s="79"/>
+      <c r="O3" s="92"/>
       <c r="P3" s="45" t="s">
         <v>163</v>
       </c>
@@ -2050,12 +2050,12 @@
       </c>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B4" s="85" t="s">
+      <c r="B4" s="73" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="86"/>
+      <c r="C4" s="74"/>
       <c r="D4" s="51">
-        <v>2.9999999999999997E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="E4" s="51" t="s">
         <v>22</v>
@@ -2066,14 +2066,14 @@
       <c r="K4" s="45" t="s">
         <v>100</v>
       </c>
-      <c r="L4" s="113"/>
+      <c r="L4" s="81"/>
       <c r="M4" s="44" t="s">
         <v>133</v>
       </c>
       <c r="N4" s="45" t="s">
         <v>134</v>
       </c>
-      <c r="O4" s="81"/>
+      <c r="O4" s="93"/>
       <c r="P4" s="45" t="s">
         <v>164</v>
       </c>
@@ -2082,10 +2082,10 @@
       </c>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B5" s="85" t="s">
+      <c r="B5" s="73" t="s">
         <v>70</v>
       </c>
-      <c r="C5" s="86"/>
+      <c r="C5" s="74"/>
       <c r="D5" s="51" t="s">
         <v>84</v>
       </c>
@@ -2098,14 +2098,14 @@
       <c r="K5" s="45" t="s">
         <v>101</v>
       </c>
-      <c r="L5" s="113"/>
+      <c r="L5" s="81"/>
       <c r="M5" s="45" t="s">
         <v>5</v>
       </c>
       <c r="N5" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="O5" s="81"/>
+      <c r="O5" s="93"/>
       <c r="P5" s="45" t="s">
         <v>165</v>
       </c>
@@ -2114,10 +2114,10 @@
       </c>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B6" s="85" t="s">
+      <c r="B6" s="73" t="s">
         <v>80</v>
       </c>
-      <c r="C6" s="86"/>
+      <c r="C6" s="74"/>
       <c r="D6" s="51" t="s">
         <v>3</v>
       </c>
@@ -2130,14 +2130,14 @@
       <c r="K6" s="45" t="s">
         <v>102</v>
       </c>
-      <c r="L6" s="113"/>
+      <c r="L6" s="81"/>
       <c r="M6" s="45" t="s">
         <v>135</v>
       </c>
       <c r="N6" s="45" t="s">
         <v>136</v>
       </c>
-      <c r="O6" s="81"/>
+      <c r="O6" s="93"/>
       <c r="P6" s="45" t="s">
         <v>169</v>
       </c>
@@ -2146,10 +2146,10 @@
       </c>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B7" s="85" t="s">
+      <c r="B7" s="73" t="s">
         <v>82</v>
       </c>
-      <c r="C7" s="86"/>
+      <c r="C7" s="74"/>
       <c r="D7" s="51">
         <v>-9806.5</v>
       </c>
@@ -2162,14 +2162,14 @@
       <c r="K7" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="L7" s="113"/>
+      <c r="L7" s="81"/>
       <c r="M7" s="45" t="s">
         <v>10</v>
       </c>
       <c r="N7" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="O7" s="81"/>
+      <c r="O7" s="93"/>
       <c r="P7" s="45" t="s">
         <v>168</v>
       </c>
@@ -2178,10 +2178,10 @@
       </c>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B8" s="85" t="s">
+      <c r="B8" s="73" t="s">
         <v>87</v>
       </c>
-      <c r="C8" s="86"/>
+      <c r="C8" s="74"/>
       <c r="D8" s="51" t="s">
         <v>131</v>
       </c>
@@ -2194,14 +2194,14 @@
       <c r="K8" s="45" t="s">
         <v>105</v>
       </c>
-      <c r="L8" s="113"/>
+      <c r="L8" s="81"/>
       <c r="M8" s="45" t="s">
         <v>12</v>
       </c>
       <c r="N8" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="O8" s="81"/>
+      <c r="O8" s="93"/>
       <c r="P8" s="45" t="s">
         <v>172</v>
       </c>
@@ -2210,10 +2210,10 @@
       </c>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B9" s="85" t="s">
+      <c r="B9" s="73" t="s">
         <v>124</v>
       </c>
-      <c r="C9" s="86"/>
+      <c r="C9" s="74"/>
       <c r="D9" s="51"/>
       <c r="E9" s="52" t="s">
         <v>125</v>
@@ -2224,14 +2224,14 @@
       <c r="K9" s="45" t="s">
         <v>103</v>
       </c>
-      <c r="L9" s="113"/>
+      <c r="L9" s="81"/>
       <c r="M9" s="45" t="s">
         <v>13</v>
       </c>
       <c r="N9" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="O9" s="81"/>
+      <c r="O9" s="93"/>
       <c r="P9" s="45" t="s">
         <v>173</v>
       </c>
@@ -2246,14 +2246,14 @@
       <c r="K10" s="32" t="s">
         <v>112</v>
       </c>
-      <c r="L10" s="113"/>
+      <c r="L10" s="81"/>
       <c r="M10" s="45" t="s">
         <v>14</v>
       </c>
       <c r="N10" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="O10" s="81"/>
+      <c r="O10" s="93"/>
       <c r="P10" s="50" t="s">
         <v>174</v>
       </c>
@@ -2264,14 +2264,14 @@
     <row r="11" spans="2:17" x14ac:dyDescent="0.25">
       <c r="J11" s="54"/>
       <c r="K11" s="55"/>
-      <c r="L11" s="113"/>
+      <c r="L11" s="81"/>
       <c r="M11" s="45" t="s">
         <v>137</v>
       </c>
       <c r="N11" s="45" t="s">
         <v>137</v>
       </c>
-      <c r="O11" s="81"/>
+      <c r="O11" s="93"/>
       <c r="P11" s="50" t="s">
         <v>175</v>
       </c>
@@ -2280,25 +2280,25 @@
       </c>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B12" s="108" t="s">
+      <c r="B12" s="71" t="s">
         <v>141</v>
       </c>
-      <c r="C12" s="108"/>
-      <c r="D12" s="108"/>
-      <c r="E12" s="108"/>
-      <c r="F12" s="108"/>
-      <c r="G12" s="108"/>
-      <c r="H12" s="108"/>
+      <c r="C12" s="71"/>
+      <c r="D12" s="71"/>
+      <c r="E12" s="71"/>
+      <c r="F12" s="71"/>
+      <c r="G12" s="71"/>
+      <c r="H12" s="71"/>
       <c r="J12" s="56"/>
       <c r="K12" s="57"/>
-      <c r="L12" s="113"/>
+      <c r="L12" s="81"/>
       <c r="M12" s="45" t="s">
         <v>138</v>
       </c>
       <c r="N12" s="45" t="s">
         <v>138</v>
       </c>
-      <c r="O12" s="81"/>
+      <c r="O12" s="93"/>
       <c r="P12" s="45" t="s">
         <v>180</v>
       </c>
@@ -2307,29 +2307,29 @@
       </c>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B13" s="84" t="s">
+      <c r="B13" s="72" t="s">
         <v>142</v>
       </c>
-      <c r="C13" s="84"/>
+      <c r="C13" s="72"/>
       <c r="D13" s="67" t="s">
         <v>241</v>
       </c>
       <c r="E13" s="67" t="s">
         <v>125</v>
       </c>
-      <c r="F13" s="89"/>
-      <c r="G13" s="89"/>
-      <c r="H13" s="89"/>
+      <c r="F13" s="96"/>
+      <c r="G13" s="96"/>
+      <c r="H13" s="96"/>
       <c r="J13" s="56"/>
       <c r="K13" s="57"/>
-      <c r="L13" s="113"/>
+      <c r="L13" s="81"/>
       <c r="M13" s="45" t="s">
         <v>19</v>
       </c>
       <c r="N13" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="O13" s="81"/>
+      <c r="O13" s="93"/>
       <c r="P13" s="50" t="s">
         <v>181</v>
       </c>
@@ -2338,27 +2338,27 @@
       </c>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B14" s="84" t="s">
+      <c r="B14" s="72" t="s">
         <v>145</v>
       </c>
-      <c r="C14" s="84"/>
+      <c r="C14" s="72"/>
       <c r="D14" s="67"/>
       <c r="E14" s="67" t="s">
         <v>125</v>
       </c>
-      <c r="F14" s="89"/>
-      <c r="G14" s="89"/>
-      <c r="H14" s="89"/>
+      <c r="F14" s="96"/>
+      <c r="G14" s="96"/>
+      <c r="H14" s="96"/>
       <c r="J14" s="58"/>
       <c r="K14" s="59"/>
-      <c r="L14" s="113"/>
+      <c r="L14" s="81"/>
       <c r="M14" s="45" t="s">
         <v>139</v>
       </c>
       <c r="N14" s="45" t="s">
         <v>139</v>
       </c>
-      <c r="O14" s="81"/>
+      <c r="O14" s="93"/>
       <c r="P14" s="50" t="s">
         <v>182</v>
       </c>
@@ -2367,31 +2367,31 @@
       </c>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B15" s="84" t="s">
+      <c r="B15" s="72" t="s">
         <v>146</v>
       </c>
-      <c r="C15" s="84"/>
+      <c r="C15" s="72"/>
       <c r="D15" s="67" t="s">
         <v>241</v>
       </c>
       <c r="E15" s="67" t="s">
         <v>125</v>
       </c>
-      <c r="F15" s="89"/>
-      <c r="G15" s="89"/>
-      <c r="H15" s="89"/>
-      <c r="J15" s="87" t="s">
+      <c r="F15" s="96"/>
+      <c r="G15" s="96"/>
+      <c r="H15" s="96"/>
+      <c r="J15" s="78" t="s">
         <v>95</v>
       </c>
-      <c r="K15" s="88"/>
-      <c r="L15" s="113"/>
+      <c r="K15" s="79"/>
+      <c r="L15" s="81"/>
       <c r="M15" s="45" t="s">
         <v>15</v>
       </c>
       <c r="N15" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="O15" s="81"/>
+      <c r="O15" s="93"/>
       <c r="P15" s="50" t="s">
         <v>183</v>
       </c>
@@ -2400,31 +2400,31 @@
       </c>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B16" s="84" t="s">
+      <c r="B16" s="72" t="s">
         <v>148</v>
       </c>
-      <c r="C16" s="84"/>
+      <c r="C16" s="72"/>
       <c r="D16" s="67"/>
       <c r="E16" s="48" t="s">
         <v>125</v>
       </c>
-      <c r="F16" s="89"/>
-      <c r="G16" s="89"/>
-      <c r="H16" s="89"/>
+      <c r="F16" s="96"/>
+      <c r="G16" s="96"/>
+      <c r="H16" s="96"/>
       <c r="J16" s="45" t="s">
         <v>96</v>
       </c>
       <c r="K16" s="45" t="s">
         <v>107</v>
       </c>
-      <c r="L16" s="113"/>
+      <c r="L16" s="81"/>
       <c r="M16" s="45" t="s">
         <v>140</v>
       </c>
       <c r="N16" s="45" t="s">
         <v>140</v>
       </c>
-      <c r="O16" s="81"/>
+      <c r="O16" s="93"/>
       <c r="P16" s="45" t="s">
         <v>188</v>
       </c>
@@ -2433,29 +2433,29 @@
       </c>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B17" s="84" t="s">
+      <c r="B17" s="72" t="s">
         <v>147</v>
       </c>
-      <c r="C17" s="84"/>
+      <c r="C17" s="72"/>
       <c r="D17" s="67"/>
       <c r="E17" s="48" t="s">
         <v>125</v>
       </c>
-      <c r="F17" s="89"/>
-      <c r="G17" s="89"/>
-      <c r="H17" s="89"/>
+      <c r="F17" s="96"/>
+      <c r="G17" s="96"/>
+      <c r="H17" s="96"/>
       <c r="J17" s="45" t="s">
         <v>0</v>
       </c>
       <c r="K17" s="45" t="s">
         <v>101</v>
       </c>
-      <c r="L17" s="113"/>
-      <c r="M17" s="87" t="s">
+      <c r="L17" s="81"/>
+      <c r="M17" s="78" t="s">
         <v>152</v>
       </c>
-      <c r="N17" s="88"/>
-      <c r="O17" s="81"/>
+      <c r="N17" s="79"/>
+      <c r="O17" s="93"/>
       <c r="P17" s="50" t="s">
         <v>189</v>
       </c>
@@ -2464,33 +2464,33 @@
       </c>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B18" s="82" t="s">
+      <c r="B18" s="94" t="s">
         <v>144</v>
       </c>
-      <c r="C18" s="83"/>
+      <c r="C18" s="95"/>
       <c r="D18" s="67" t="s">
         <v>241</v>
       </c>
       <c r="E18" s="48" t="s">
         <v>125</v>
       </c>
-      <c r="F18" s="89"/>
-      <c r="G18" s="89"/>
-      <c r="H18" s="89"/>
+      <c r="F18" s="96"/>
+      <c r="G18" s="96"/>
+      <c r="H18" s="96"/>
       <c r="J18" s="45" t="s">
         <v>97</v>
       </c>
       <c r="K18" s="45" t="s">
         <v>102</v>
       </c>
-      <c r="L18" s="113"/>
+      <c r="L18" s="81"/>
       <c r="M18" s="53" t="s">
         <v>162</v>
       </c>
       <c r="N18" s="32" t="s">
         <v>134</v>
       </c>
-      <c r="O18" s="81"/>
+      <c r="O18" s="93"/>
       <c r="P18" s="50" t="s">
         <v>190</v>
       </c>
@@ -2499,31 +2499,31 @@
       </c>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B19" s="82" t="s">
+      <c r="B19" s="94" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="83"/>
+      <c r="C19" s="95"/>
       <c r="D19" s="67"/>
       <c r="E19" s="48" t="s">
         <v>125</v>
       </c>
-      <c r="F19" s="89"/>
-      <c r="G19" s="89"/>
-      <c r="H19" s="89"/>
+      <c r="F19" s="96"/>
+      <c r="G19" s="96"/>
+      <c r="H19" s="96"/>
       <c r="J19" s="45" t="s">
         <v>98</v>
       </c>
       <c r="K19" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="L19" s="113"/>
+      <c r="L19" s="81"/>
       <c r="M19" s="46" t="s">
         <v>153</v>
       </c>
       <c r="N19" s="46" t="s">
         <v>72</v>
       </c>
-      <c r="O19" s="81"/>
+      <c r="O19" s="93"/>
       <c r="P19" s="50" t="s">
         <v>191</v>
       </c>
@@ -2532,33 +2532,33 @@
       </c>
     </row>
     <row r="20" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="71" t="s">
+      <c r="B20" s="83" t="s">
         <v>250</v>
       </c>
-      <c r="C20" s="73"/>
+      <c r="C20" s="85"/>
       <c r="D20" s="48" t="s">
         <v>241</v>
       </c>
       <c r="E20" s="48" t="s">
         <v>125</v>
       </c>
-      <c r="F20" s="89"/>
-      <c r="G20" s="89"/>
-      <c r="H20" s="89"/>
+      <c r="F20" s="96"/>
+      <c r="G20" s="96"/>
+      <c r="H20" s="96"/>
       <c r="J20" s="45" t="s">
         <v>104</v>
       </c>
       <c r="K20" s="45" t="s">
         <v>108</v>
       </c>
-      <c r="L20" s="113"/>
+      <c r="L20" s="81"/>
       <c r="M20" s="46" t="s">
         <v>154</v>
       </c>
       <c r="N20" s="46" t="s">
         <v>73</v>
       </c>
-      <c r="O20" s="81"/>
+      <c r="O20" s="93"/>
       <c r="P20" s="45" t="s">
         <v>196</v>
       </c>
@@ -2567,31 +2567,31 @@
       </c>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B21" s="84" t="s">
+      <c r="B21" s="72" t="s">
         <v>251</v>
       </c>
-      <c r="C21" s="84"/>
+      <c r="C21" s="72"/>
       <c r="D21" s="49"/>
       <c r="E21" s="67" t="s">
         <v>125</v>
       </c>
-      <c r="F21" s="89"/>
-      <c r="G21" s="89"/>
-      <c r="H21" s="89"/>
+      <c r="F21" s="96"/>
+      <c r="G21" s="96"/>
+      <c r="H21" s="96"/>
       <c r="J21" s="45" t="s">
         <v>99</v>
       </c>
       <c r="K21" s="45" t="s">
         <v>103</v>
       </c>
-      <c r="L21" s="113"/>
+      <c r="L21" s="81"/>
       <c r="M21" s="46" t="s">
         <v>155</v>
       </c>
       <c r="N21" s="46" t="s">
         <v>159</v>
       </c>
-      <c r="O21" s="81"/>
+      <c r="O21" s="93"/>
       <c r="P21" s="50" t="s">
         <v>197</v>
       </c>
@@ -2600,35 +2600,35 @@
       </c>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B22" s="90" t="s">
+      <c r="B22" s="97" t="s">
         <v>143</v>
       </c>
-      <c r="C22" s="91"/>
+      <c r="C22" s="98"/>
       <c r="D22" s="67">
         <v>2</v>
       </c>
-      <c r="E22" s="96" t="s">
+      <c r="E22" s="103" t="s">
         <v>149</v>
       </c>
-      <c r="F22" s="99" t="s">
+      <c r="F22" s="106" t="s">
         <v>150</v>
       </c>
-      <c r="G22" s="100"/>
-      <c r="H22" s="101"/>
+      <c r="G22" s="107"/>
+      <c r="H22" s="108"/>
       <c r="J22" s="32" t="s">
         <v>110</v>
       </c>
       <c r="K22" s="32" t="s">
         <v>111</v>
       </c>
-      <c r="L22" s="114"/>
+      <c r="L22" s="82"/>
       <c r="M22" s="46" t="s">
         <v>156</v>
       </c>
       <c r="N22" s="45" t="s">
         <v>158</v>
       </c>
-      <c r="O22" s="81"/>
+      <c r="O22" s="93"/>
       <c r="P22" s="50" t="s">
         <v>198</v>
       </c>
@@ -2637,21 +2637,21 @@
       </c>
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B23" s="92"/>
-      <c r="C23" s="93"/>
+      <c r="B23" s="99"/>
+      <c r="C23" s="100"/>
       <c r="D23" s="67">
         <v>3</v>
       </c>
-      <c r="E23" s="97"/>
-      <c r="F23" s="102"/>
-      <c r="G23" s="103"/>
-      <c r="H23" s="104"/>
-      <c r="J23" s="71"/>
-      <c r="K23" s="72"/>
-      <c r="L23" s="72"/>
-      <c r="M23" s="72"/>
-      <c r="N23" s="73"/>
-      <c r="O23" s="81"/>
+      <c r="E23" s="104"/>
+      <c r="F23" s="109"/>
+      <c r="G23" s="110"/>
+      <c r="H23" s="111"/>
+      <c r="J23" s="83"/>
+      <c r="K23" s="84"/>
+      <c r="L23" s="84"/>
+      <c r="M23" s="84"/>
+      <c r="N23" s="85"/>
+      <c r="O23" s="93"/>
       <c r="P23" s="50" t="s">
         <v>199</v>
       </c>
@@ -2660,19 +2660,19 @@
       </c>
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B24" s="92"/>
-      <c r="C24" s="93"/>
+      <c r="B24" s="99"/>
+      <c r="C24" s="100"/>
       <c r="D24" s="67"/>
-      <c r="E24" s="97"/>
-      <c r="F24" s="102"/>
-      <c r="G24" s="103"/>
-      <c r="H24" s="104"/>
-      <c r="J24" s="74"/>
-      <c r="K24" s="75"/>
-      <c r="L24" s="75"/>
-      <c r="M24" s="75"/>
-      <c r="N24" s="76"/>
-      <c r="O24" s="81"/>
+      <c r="E24" s="104"/>
+      <c r="F24" s="109"/>
+      <c r="G24" s="110"/>
+      <c r="H24" s="111"/>
+      <c r="J24" s="86"/>
+      <c r="K24" s="87"/>
+      <c r="L24" s="87"/>
+      <c r="M24" s="87"/>
+      <c r="N24" s="88"/>
+      <c r="O24" s="93"/>
       <c r="P24" s="32" t="s">
         <v>205</v>
       </c>
@@ -2681,19 +2681,19 @@
       </c>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B25" s="92"/>
-      <c r="C25" s="93"/>
+      <c r="B25" s="99"/>
+      <c r="C25" s="100"/>
       <c r="D25" s="67"/>
-      <c r="E25" s="97"/>
-      <c r="F25" s="102"/>
-      <c r="G25" s="103"/>
-      <c r="H25" s="104"/>
-      <c r="J25" s="74"/>
-      <c r="K25" s="75"/>
-      <c r="L25" s="75"/>
-      <c r="M25" s="75"/>
-      <c r="N25" s="76"/>
-      <c r="O25" s="81"/>
+      <c r="E25" s="104"/>
+      <c r="F25" s="109"/>
+      <c r="G25" s="110"/>
+      <c r="H25" s="111"/>
+      <c r="J25" s="86"/>
+      <c r="K25" s="87"/>
+      <c r="L25" s="87"/>
+      <c r="M25" s="87"/>
+      <c r="N25" s="88"/>
+      <c r="O25" s="93"/>
       <c r="P25" s="32" t="s">
         <v>209</v>
       </c>
@@ -2702,19 +2702,19 @@
       </c>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B26" s="92"/>
-      <c r="C26" s="93"/>
+      <c r="B26" s="99"/>
+      <c r="C26" s="100"/>
       <c r="D26" s="67"/>
-      <c r="E26" s="97"/>
-      <c r="F26" s="102"/>
-      <c r="G26" s="103"/>
-      <c r="H26" s="104"/>
-      <c r="J26" s="74"/>
-      <c r="K26" s="75"/>
-      <c r="L26" s="75"/>
-      <c r="M26" s="75"/>
-      <c r="N26" s="76"/>
-      <c r="O26" s="81"/>
+      <c r="E26" s="104"/>
+      <c r="F26" s="109"/>
+      <c r="G26" s="110"/>
+      <c r="H26" s="111"/>
+      <c r="J26" s="86"/>
+      <c r="K26" s="87"/>
+      <c r="L26" s="87"/>
+      <c r="M26" s="87"/>
+      <c r="N26" s="88"/>
+      <c r="O26" s="93"/>
       <c r="P26" s="32" t="s">
         <v>210</v>
       </c>
@@ -2723,19 +2723,19 @@
       </c>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B27" s="92"/>
-      <c r="C27" s="93"/>
+      <c r="B27" s="99"/>
+      <c r="C27" s="100"/>
       <c r="D27" s="67"/>
-      <c r="E27" s="97"/>
-      <c r="F27" s="102"/>
-      <c r="G27" s="103"/>
-      <c r="H27" s="104"/>
-      <c r="J27" s="74"/>
-      <c r="K27" s="75"/>
-      <c r="L27" s="75"/>
-      <c r="M27" s="75"/>
-      <c r="N27" s="76"/>
-      <c r="O27" s="81"/>
+      <c r="E27" s="104"/>
+      <c r="F27" s="109"/>
+      <c r="G27" s="110"/>
+      <c r="H27" s="111"/>
+      <c r="J27" s="86"/>
+      <c r="K27" s="87"/>
+      <c r="L27" s="87"/>
+      <c r="M27" s="87"/>
+      <c r="N27" s="88"/>
+      <c r="O27" s="93"/>
       <c r="P27" s="32" t="s">
         <v>211</v>
       </c>
@@ -2744,19 +2744,19 @@
       </c>
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B28" s="92"/>
-      <c r="C28" s="93"/>
+      <c r="B28" s="99"/>
+      <c r="C28" s="100"/>
       <c r="D28" s="67"/>
-      <c r="E28" s="97"/>
-      <c r="F28" s="102"/>
-      <c r="G28" s="103"/>
-      <c r="H28" s="104"/>
-      <c r="J28" s="74"/>
-      <c r="K28" s="75"/>
-      <c r="L28" s="75"/>
-      <c r="M28" s="75"/>
-      <c r="N28" s="76"/>
-      <c r="O28" s="81"/>
+      <c r="E28" s="104"/>
+      <c r="F28" s="109"/>
+      <c r="G28" s="110"/>
+      <c r="H28" s="111"/>
+      <c r="J28" s="86"/>
+      <c r="K28" s="87"/>
+      <c r="L28" s="87"/>
+      <c r="M28" s="87"/>
+      <c r="N28" s="88"/>
+      <c r="O28" s="93"/>
       <c r="P28" s="32" t="s">
         <v>213</v>
       </c>
@@ -2765,19 +2765,19 @@
       </c>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B29" s="94"/>
-      <c r="C29" s="95"/>
+      <c r="B29" s="101"/>
+      <c r="C29" s="102"/>
       <c r="D29" s="67"/>
-      <c r="E29" s="98"/>
-      <c r="F29" s="105"/>
-      <c r="G29" s="106"/>
-      <c r="H29" s="107"/>
-      <c r="J29" s="74"/>
-      <c r="K29" s="75"/>
-      <c r="L29" s="75"/>
-      <c r="M29" s="75"/>
-      <c r="N29" s="76"/>
-      <c r="O29" s="81"/>
+      <c r="E29" s="105"/>
+      <c r="F29" s="112"/>
+      <c r="G29" s="113"/>
+      <c r="H29" s="114"/>
+      <c r="J29" s="86"/>
+      <c r="K29" s="87"/>
+      <c r="L29" s="87"/>
+      <c r="M29" s="87"/>
+      <c r="N29" s="88"/>
+      <c r="O29" s="93"/>
       <c r="P29" s="32" t="s">
         <v>212</v>
       </c>
@@ -2786,12 +2786,12 @@
       </c>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="J30" s="74"/>
-      <c r="K30" s="75"/>
-      <c r="L30" s="75"/>
-      <c r="M30" s="75"/>
-      <c r="N30" s="76"/>
-      <c r="O30" s="81"/>
+      <c r="J30" s="86"/>
+      <c r="K30" s="87"/>
+      <c r="L30" s="87"/>
+      <c r="M30" s="87"/>
+      <c r="N30" s="88"/>
+      <c r="O30" s="93"/>
       <c r="P30" s="32" t="s">
         <v>214</v>
       </c>
@@ -2800,12 +2800,12 @@
       </c>
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="J31" s="74"/>
-      <c r="K31" s="75"/>
-      <c r="L31" s="75"/>
-      <c r="M31" s="75"/>
-      <c r="N31" s="76"/>
-      <c r="O31" s="81"/>
+      <c r="J31" s="86"/>
+      <c r="K31" s="87"/>
+      <c r="L31" s="87"/>
+      <c r="M31" s="87"/>
+      <c r="N31" s="88"/>
+      <c r="O31" s="93"/>
       <c r="P31" s="32" t="s">
         <v>215</v>
       </c>
@@ -2814,12 +2814,12 @@
       </c>
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="J32" s="74"/>
-      <c r="K32" s="75"/>
-      <c r="L32" s="75"/>
-      <c r="M32" s="75"/>
-      <c r="N32" s="76"/>
-      <c r="O32" s="81"/>
+      <c r="J32" s="86"/>
+      <c r="K32" s="87"/>
+      <c r="L32" s="87"/>
+      <c r="M32" s="87"/>
+      <c r="N32" s="88"/>
+      <c r="O32" s="93"/>
       <c r="P32" s="32" t="s">
         <v>216</v>
       </c>
@@ -2828,12 +2828,12 @@
       </c>
     </row>
     <row r="33" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J33" s="74"/>
-      <c r="K33" s="75"/>
-      <c r="L33" s="75"/>
-      <c r="M33" s="75"/>
-      <c r="N33" s="76"/>
-      <c r="O33" s="81"/>
+      <c r="J33" s="86"/>
+      <c r="K33" s="87"/>
+      <c r="L33" s="87"/>
+      <c r="M33" s="87"/>
+      <c r="N33" s="88"/>
+      <c r="O33" s="93"/>
       <c r="P33" s="32" t="s">
         <v>217</v>
       </c>
@@ -2842,12 +2842,12 @@
       </c>
     </row>
     <row r="34" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J34" s="74"/>
-      <c r="K34" s="75"/>
-      <c r="L34" s="75"/>
-      <c r="M34" s="75"/>
-      <c r="N34" s="76"/>
-      <c r="O34" s="81"/>
+      <c r="J34" s="86"/>
+      <c r="K34" s="87"/>
+      <c r="L34" s="87"/>
+      <c r="M34" s="87"/>
+      <c r="N34" s="88"/>
+      <c r="O34" s="93"/>
       <c r="P34" s="32" t="s">
         <v>218</v>
       </c>
@@ -2856,12 +2856,12 @@
       </c>
     </row>
     <row r="35" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J35" s="74"/>
-      <c r="K35" s="75"/>
-      <c r="L35" s="75"/>
-      <c r="M35" s="75"/>
-      <c r="N35" s="76"/>
-      <c r="O35" s="81"/>
+      <c r="J35" s="86"/>
+      <c r="K35" s="87"/>
+      <c r="L35" s="87"/>
+      <c r="M35" s="87"/>
+      <c r="N35" s="88"/>
+      <c r="O35" s="93"/>
       <c r="P35" s="32" t="s">
         <v>219</v>
       </c>
@@ -2870,12 +2870,12 @@
       </c>
     </row>
     <row r="36" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J36" s="74"/>
-      <c r="K36" s="75"/>
-      <c r="L36" s="75"/>
-      <c r="M36" s="75"/>
-      <c r="N36" s="76"/>
-      <c r="O36" s="81"/>
+      <c r="J36" s="86"/>
+      <c r="K36" s="87"/>
+      <c r="L36" s="87"/>
+      <c r="M36" s="87"/>
+      <c r="N36" s="88"/>
+      <c r="O36" s="93"/>
       <c r="P36" s="32" t="s">
         <v>228</v>
       </c>
@@ -2884,12 +2884,12 @@
       </c>
     </row>
     <row r="37" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J37" s="74"/>
-      <c r="K37" s="75"/>
-      <c r="L37" s="75"/>
-      <c r="M37" s="75"/>
-      <c r="N37" s="76"/>
-      <c r="O37" s="81"/>
+      <c r="J37" s="86"/>
+      <c r="K37" s="87"/>
+      <c r="L37" s="87"/>
+      <c r="M37" s="87"/>
+      <c r="N37" s="88"/>
+      <c r="O37" s="93"/>
       <c r="P37" s="32" t="s">
         <v>229</v>
       </c>
@@ -2898,12 +2898,12 @@
       </c>
     </row>
     <row r="38" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J38" s="77"/>
-      <c r="K38" s="78"/>
-      <c r="L38" s="78"/>
-      <c r="M38" s="78"/>
-      <c r="N38" s="79"/>
-      <c r="O38" s="81"/>
+      <c r="J38" s="89"/>
+      <c r="K38" s="90"/>
+      <c r="L38" s="90"/>
+      <c r="M38" s="90"/>
+      <c r="N38" s="91"/>
+      <c r="O38" s="93"/>
       <c r="P38" s="32" t="s">
         <v>230</v>
       </c>
@@ -2921,6 +2921,21 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="J23:N38"/>
+    <mergeCell ref="O3:O38"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="F13:H21"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C29"/>
+    <mergeCell ref="E22:E29"/>
+    <mergeCell ref="F22:H29"/>
     <mergeCell ref="J2:Q2"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B14:C14"/>
@@ -2936,21 +2951,6 @@
     <mergeCell ref="L3:L22"/>
     <mergeCell ref="J15:K15"/>
     <mergeCell ref="M17:N17"/>
-    <mergeCell ref="J23:N38"/>
-    <mergeCell ref="O3:O38"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="F13:H21"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C29"/>
-    <mergeCell ref="E22:E29"/>
-    <mergeCell ref="F22:H29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2962,8 +2962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK197"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U17" sqref="U17"/>
+    <sheetView topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AA7" sqref="AA7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2982,118 +2982,118 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A1" s="89"/>
-      <c r="B1" s="89"/>
-      <c r="C1" s="84" t="s">
+      <c r="A1" s="96"/>
+      <c r="B1" s="96"/>
+      <c r="C1" s="72" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84" t="s">
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="84"/>
-      <c r="H1" s="84"/>
-      <c r="I1" s="84"/>
-      <c r="J1" s="84"/>
-      <c r="K1" s="84"/>
-      <c r="L1" s="84" t="s">
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="72"/>
+      <c r="K1" s="72"/>
+      <c r="L1" s="72" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="84"/>
-      <c r="N1" s="84"/>
-      <c r="O1" s="84" t="s">
+      <c r="M1" s="72"/>
+      <c r="N1" s="72"/>
+      <c r="O1" s="72" t="s">
         <v>41</v>
       </c>
-      <c r="P1" s="84"/>
-      <c r="Q1" s="84"/>
-      <c r="R1" s="84"/>
-      <c r="S1" s="84" t="s">
+      <c r="P1" s="72"/>
+      <c r="Q1" s="72"/>
+      <c r="R1" s="72"/>
+      <c r="S1" s="72" t="s">
         <v>34</v>
       </c>
-      <c r="T1" s="84"/>
-      <c r="U1" s="84"/>
-      <c r="V1" s="84"/>
-      <c r="W1" s="84"/>
-      <c r="X1" s="84"/>
-      <c r="Y1" s="84"/>
-      <c r="Z1" s="84"/>
-      <c r="AA1" s="84"/>
-      <c r="AB1" s="84"/>
-      <c r="AC1" s="84"/>
-      <c r="AD1" s="84"/>
-      <c r="AE1" s="84"/>
-      <c r="AF1" s="84"/>
-      <c r="AG1" s="84"/>
-      <c r="AH1" s="84"/>
-      <c r="AI1" s="84"/>
-      <c r="AJ1" s="84"/>
-      <c r="AK1" s="84"/>
+      <c r="T1" s="72"/>
+      <c r="U1" s="72"/>
+      <c r="V1" s="72"/>
+      <c r="W1" s="72"/>
+      <c r="X1" s="72"/>
+      <c r="Y1" s="72"/>
+      <c r="Z1" s="72"/>
+      <c r="AA1" s="72"/>
+      <c r="AB1" s="72"/>
+      <c r="AC1" s="72"/>
+      <c r="AD1" s="72"/>
+      <c r="AE1" s="72"/>
+      <c r="AF1" s="72"/>
+      <c r="AG1" s="72"/>
+      <c r="AH1" s="72"/>
+      <c r="AI1" s="72"/>
+      <c r="AJ1" s="72"/>
+      <c r="AK1" s="72"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A2" s="89"/>
-      <c r="B2" s="89"/>
-      <c r="C2" s="117" t="s">
+      <c r="A2" s="96"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="116" t="s">
         <v>75</v>
       </c>
-      <c r="D2" s="117"/>
-      <c r="E2" s="117"/>
-      <c r="F2" s="117" t="s">
+      <c r="D2" s="116"/>
+      <c r="E2" s="116"/>
+      <c r="F2" s="116" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="117"/>
-      <c r="H2" s="117"/>
-      <c r="I2" s="117" t="s">
+      <c r="G2" s="116"/>
+      <c r="H2" s="116"/>
+      <c r="I2" s="116" t="s">
         <v>29</v>
       </c>
-      <c r="J2" s="117"/>
-      <c r="K2" s="117"/>
-      <c r="L2" s="84" t="s">
+      <c r="J2" s="116"/>
+      <c r="K2" s="116"/>
+      <c r="L2" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="M2" s="84"/>
-      <c r="N2" s="84"/>
-      <c r="O2" s="84" t="s">
+      <c r="M2" s="72"/>
+      <c r="N2" s="72"/>
+      <c r="O2" s="72" t="s">
         <v>38</v>
       </c>
-      <c r="P2" s="84"/>
-      <c r="Q2" s="84"/>
-      <c r="R2" s="118" t="s">
+      <c r="P2" s="72"/>
+      <c r="Q2" s="72"/>
+      <c r="R2" s="117" t="s">
         <v>86</v>
       </c>
-      <c r="S2" s="116" t="s">
-        <v>0</v>
-      </c>
-      <c r="T2" s="117" t="s">
+      <c r="S2" s="115" t="s">
+        <v>0</v>
+      </c>
+      <c r="T2" s="116" t="s">
         <v>94</v>
       </c>
-      <c r="U2" s="117"/>
-      <c r="V2" s="117"/>
-      <c r="W2" s="84" t="s">
+      <c r="U2" s="116"/>
+      <c r="V2" s="116"/>
+      <c r="W2" s="72" t="s">
         <v>92</v>
       </c>
-      <c r="X2" s="84"/>
-      <c r="Y2" s="84"/>
-      <c r="Z2" s="82" t="s">
+      <c r="X2" s="72"/>
+      <c r="Y2" s="72"/>
+      <c r="Z2" s="94" t="s">
         <v>93</v>
       </c>
-      <c r="AA2" s="115"/>
-      <c r="AB2" s="83"/>
-      <c r="AC2" s="84" t="s">
+      <c r="AA2" s="118"/>
+      <c r="AB2" s="95"/>
+      <c r="AC2" s="72" t="s">
         <v>90</v>
       </c>
-      <c r="AD2" s="84"/>
-      <c r="AE2" s="84"/>
-      <c r="AF2" s="84" t="s">
+      <c r="AD2" s="72"/>
+      <c r="AE2" s="72"/>
+      <c r="AF2" s="72" t="s">
         <v>91</v>
       </c>
-      <c r="AG2" s="84"/>
-      <c r="AH2" s="84"/>
-      <c r="AI2" s="84" t="s">
+      <c r="AG2" s="72"/>
+      <c r="AH2" s="72"/>
+      <c r="AI2" s="72" t="s">
         <v>76</v>
       </c>
-      <c r="AJ2" s="84"/>
-      <c r="AK2" s="84"/>
+      <c r="AJ2" s="72"/>
+      <c r="AK2" s="72"/>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
@@ -3147,8 +3147,8 @@
       <c r="Q3" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="R3" s="118"/>
-      <c r="S3" s="116"/>
+      <c r="R3" s="117"/>
+      <c r="S3" s="115"/>
       <c r="T3" s="16" t="s">
         <v>62</v>
       </c>
@@ -3598,7 +3598,7 @@
         <v>1</v>
       </c>
       <c r="R7" s="30">
-        <v>0.52359900000000004</v>
+        <v>-0.52359900000000004</v>
       </c>
       <c r="S7" s="16">
         <v>6.2439999999999998</v>
@@ -3714,7 +3714,7 @@
         <v>1</v>
       </c>
       <c r="R8" s="63">
-        <v>-0.52359900000000004</v>
+        <v>0.52359900000000004</v>
       </c>
       <c r="S8" s="63">
         <v>6.2439999999999998</v>
@@ -6834,6 +6834,12 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="W2:Y2"/>
+    <mergeCell ref="AC2:AE2"/>
+    <mergeCell ref="AF2:AH2"/>
+    <mergeCell ref="AI2:AK2"/>
+    <mergeCell ref="S1:AK1"/>
+    <mergeCell ref="Z2:AB2"/>
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="S2:S3"/>
     <mergeCell ref="T2:V2"/>
@@ -6847,12 +6853,6 @@
     <mergeCell ref="L2:N2"/>
     <mergeCell ref="L1:N1"/>
     <mergeCell ref="C1:E1"/>
-    <mergeCell ref="W2:Y2"/>
-    <mergeCell ref="AC2:AE2"/>
-    <mergeCell ref="AF2:AH2"/>
-    <mergeCell ref="AI2:AK2"/>
-    <mergeCell ref="S1:AK1"/>
-    <mergeCell ref="Z2:AB2"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -6884,16 +6884,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="120" t="s">
+      <c r="A1" s="119" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="120"/>
-      <c r="C1" s="120"/>
-      <c r="D1" s="120"/>
-      <c r="E1" s="120"/>
-      <c r="F1" s="120"/>
-      <c r="G1" s="120"/>
-      <c r="H1" s="120"/>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="119"/>
+      <c r="F1" s="119"/>
+      <c r="G1" s="119"/>
+      <c r="H1" s="119"/>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
@@ -6924,11 +6924,11 @@
       <c r="E2" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="121" t="s">
+      <c r="F2" s="120" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="121"/>
-      <c r="H2" s="121"/>
+      <c r="G2" s="120"/>
+      <c r="H2" s="120"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -6984,19 +6984,19 @@
       <c r="X4" s="10"/>
     </row>
     <row r="5" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="120" t="s">
+      <c r="A5" s="119" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="120"/>
-      <c r="C5" s="120"/>
-      <c r="D5" s="120"/>
-      <c r="E5" s="120"/>
-      <c r="F5" s="120"/>
-      <c r="G5" s="120"/>
-      <c r="H5" s="120"/>
-      <c r="I5" s="120"/>
-      <c r="J5" s="120"/>
-      <c r="K5" s="120"/>
+      <c r="B5" s="119"/>
+      <c r="C5" s="119"/>
+      <c r="D5" s="119"/>
+      <c r="E5" s="119"/>
+      <c r="F5" s="119"/>
+      <c r="G5" s="119"/>
+      <c r="H5" s="119"/>
+      <c r="I5" s="119"/>
+      <c r="J5" s="119"/>
+      <c r="K5" s="119"/>
       <c r="R5" s="10"/>
       <c r="S5" s="10"/>
       <c r="T5" s="10"/>
@@ -7021,16 +7021,16 @@
       <c r="E6" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="125" t="s">
+      <c r="F6" s="122" t="s">
         <v>47</v>
       </c>
-      <c r="G6" s="126"/>
-      <c r="H6" s="127"/>
-      <c r="I6" s="125" t="s">
+      <c r="G6" s="123"/>
+      <c r="H6" s="124"/>
+      <c r="I6" s="122" t="s">
         <v>48</v>
       </c>
-      <c r="J6" s="126"/>
-      <c r="K6" s="127"/>
+      <c r="J6" s="123"/>
+      <c r="K6" s="124"/>
       <c r="L6" s="20"/>
       <c r="M6" s="20"/>
       <c r="N6" s="20"/>
@@ -7066,22 +7066,22 @@
       <c r="X7" s="10"/>
     </row>
     <row r="8" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="120" t="s">
+      <c r="A8" s="119" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="120"/>
-      <c r="C8" s="120"/>
-      <c r="D8" s="120"/>
-      <c r="E8" s="120"/>
-      <c r="F8" s="120"/>
-      <c r="G8" s="120"/>
-      <c r="H8" s="120"/>
-      <c r="I8" s="120"/>
-      <c r="J8" s="120"/>
-      <c r="K8" s="120"/>
-      <c r="L8" s="120"/>
-      <c r="M8" s="120"/>
-      <c r="N8" s="120"/>
+      <c r="B8" s="119"/>
+      <c r="C8" s="119"/>
+      <c r="D8" s="119"/>
+      <c r="E8" s="119"/>
+      <c r="F8" s="119"/>
+      <c r="G8" s="119"/>
+      <c r="H8" s="119"/>
+      <c r="I8" s="119"/>
+      <c r="J8" s="119"/>
+      <c r="K8" s="119"/>
+      <c r="L8" s="119"/>
+      <c r="M8" s="119"/>
+      <c r="N8" s="119"/>
       <c r="R8" s="10"/>
       <c r="S8" s="10"/>
       <c r="T8" s="10"/>
@@ -7106,21 +7106,21 @@
       <c r="E9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="121" t="s">
+      <c r="F9" s="120" t="s">
         <v>42</v>
       </c>
-      <c r="G9" s="121"/>
-      <c r="H9" s="121"/>
-      <c r="I9" s="119" t="s">
+      <c r="G9" s="120"/>
+      <c r="H9" s="120"/>
+      <c r="I9" s="121" t="s">
         <v>43</v>
       </c>
-      <c r="J9" s="119"/>
-      <c r="K9" s="119"/>
-      <c r="L9" s="119" t="s">
+      <c r="J9" s="121"/>
+      <c r="K9" s="121"/>
+      <c r="L9" s="121" t="s">
         <v>44</v>
       </c>
-      <c r="M9" s="119"/>
-      <c r="N9" s="119"/>
+      <c r="M9" s="121"/>
+      <c r="N9" s="121"/>
       <c r="R9" s="10"/>
       <c r="S9" s="10"/>
       <c r="T9" s="10"/>
@@ -7174,19 +7174,19 @@
       <c r="X11" s="10"/>
     </row>
     <row r="12" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="120" t="s">
+      <c r="A12" s="119" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="120"/>
-      <c r="C12" s="120"/>
-      <c r="D12" s="120"/>
-      <c r="E12" s="120"/>
-      <c r="F12" s="120"/>
-      <c r="G12" s="120"/>
-      <c r="H12" s="120"/>
-      <c r="I12" s="120"/>
-      <c r="J12" s="120"/>
-      <c r="K12" s="120"/>
+      <c r="B12" s="119"/>
+      <c r="C12" s="119"/>
+      <c r="D12" s="119"/>
+      <c r="E12" s="119"/>
+      <c r="F12" s="119"/>
+      <c r="G12" s="119"/>
+      <c r="H12" s="119"/>
+      <c r="I12" s="119"/>
+      <c r="J12" s="119"/>
+      <c r="K12" s="119"/>
       <c r="R12" s="10"/>
       <c r="S12" s="10"/>
       <c r="T12" s="10"/>
@@ -7211,16 +7211,16 @@
       <c r="E13" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="121" t="s">
+      <c r="F13" s="120" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="121"/>
-      <c r="H13" s="121"/>
-      <c r="I13" s="119" t="s">
+      <c r="G13" s="120"/>
+      <c r="H13" s="120"/>
+      <c r="I13" s="121" t="s">
         <v>45</v>
       </c>
-      <c r="J13" s="119"/>
-      <c r="K13" s="119"/>
+      <c r="J13" s="121"/>
+      <c r="K13" s="121"/>
       <c r="R13" s="10"/>
       <c r="S13" s="10"/>
       <c r="T13" s="10"/>
@@ -7362,19 +7362,19 @@
       <c r="X17" s="10"/>
     </row>
     <row r="18" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A18" s="120" t="s">
+      <c r="A18" s="119" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="120"/>
-      <c r="C18" s="120"/>
-      <c r="D18" s="120"/>
-      <c r="E18" s="120"/>
-      <c r="F18" s="120"/>
-      <c r="G18" s="120"/>
-      <c r="H18" s="120"/>
-      <c r="I18" s="120"/>
-      <c r="J18" s="120"/>
-      <c r="K18" s="120"/>
+      <c r="B18" s="119"/>
+      <c r="C18" s="119"/>
+      <c r="D18" s="119"/>
+      <c r="E18" s="119"/>
+      <c r="F18" s="119"/>
+      <c r="G18" s="119"/>
+      <c r="H18" s="119"/>
+      <c r="I18" s="119"/>
+      <c r="J18" s="119"/>
+      <c r="K18" s="119"/>
       <c r="R18" s="10"/>
       <c r="S18" s="10"/>
       <c r="T18" s="10"/>
@@ -7399,16 +7399,16 @@
       <c r="E19" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="121" t="s">
+      <c r="F19" s="120" t="s">
         <v>42</v>
       </c>
-      <c r="G19" s="121"/>
-      <c r="H19" s="121"/>
-      <c r="I19" s="119" t="s">
+      <c r="G19" s="120"/>
+      <c r="H19" s="120"/>
+      <c r="I19" s="121" t="s">
         <v>43</v>
       </c>
-      <c r="J19" s="119"/>
-      <c r="K19" s="119"/>
+      <c r="J19" s="121"/>
+      <c r="K19" s="121"/>
     </row>
     <row r="20" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="18"/>
@@ -7445,19 +7445,19 @@
       <c r="X21" s="10"/>
     </row>
     <row r="22" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A22" s="120" t="s">
+      <c r="A22" s="119" t="s">
         <v>14</v>
       </c>
-      <c r="B22" s="120"/>
-      <c r="C22" s="120"/>
-      <c r="D22" s="120"/>
-      <c r="E22" s="120"/>
-      <c r="F22" s="120"/>
-      <c r="G22" s="120"/>
-      <c r="H22" s="120"/>
-      <c r="I22" s="120"/>
-      <c r="J22" s="120"/>
-      <c r="K22" s="120"/>
+      <c r="B22" s="119"/>
+      <c r="C22" s="119"/>
+      <c r="D22" s="119"/>
+      <c r="E22" s="119"/>
+      <c r="F22" s="119"/>
+      <c r="G22" s="119"/>
+      <c r="H22" s="119"/>
+      <c r="I22" s="119"/>
+      <c r="J22" s="119"/>
+      <c r="K22" s="119"/>
       <c r="R22" s="10"/>
       <c r="S22" s="10"/>
       <c r="T22" s="10"/>
@@ -7482,16 +7482,16 @@
       <c r="E23" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="F23" s="121" t="s">
+      <c r="F23" s="120" t="s">
         <v>42</v>
       </c>
-      <c r="G23" s="121"/>
-      <c r="H23" s="121"/>
-      <c r="I23" s="119" t="s">
+      <c r="G23" s="120"/>
+      <c r="H23" s="120"/>
+      <c r="I23" s="121" t="s">
         <v>11</v>
       </c>
-      <c r="J23" s="119"/>
-      <c r="K23" s="119"/>
+      <c r="J23" s="121"/>
+      <c r="K23" s="121"/>
     </row>
     <row r="24" spans="1:24" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="18">
@@ -7527,22 +7527,22 @@
     </row>
     <row r="25" spans="1:24" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="1:24" s="18" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A26" s="120" t="s">
+      <c r="A26" s="119" t="s">
         <v>126</v>
       </c>
-      <c r="B26" s="120"/>
-      <c r="C26" s="120"/>
-      <c r="D26" s="120"/>
-      <c r="E26" s="120"/>
-      <c r="F26" s="120"/>
-      <c r="G26" s="120"/>
-      <c r="H26" s="120"/>
-      <c r="I26" s="120"/>
-      <c r="J26" s="120"/>
-      <c r="K26" s="120"/>
-      <c r="L26" s="120"/>
-      <c r="M26" s="120"/>
-      <c r="N26" s="120"/>
+      <c r="B26" s="119"/>
+      <c r="C26" s="119"/>
+      <c r="D26" s="119"/>
+      <c r="E26" s="119"/>
+      <c r="F26" s="119"/>
+      <c r="G26" s="119"/>
+      <c r="H26" s="119"/>
+      <c r="I26" s="119"/>
+      <c r="J26" s="119"/>
+      <c r="K26" s="119"/>
+      <c r="L26" s="119"/>
+      <c r="M26" s="119"/>
+      <c r="N26" s="119"/>
     </row>
     <row r="27" spans="1:24" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="37" t="s">
@@ -7560,44 +7560,44 @@
       <c r="E27" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="F27" s="121" t="s">
+      <c r="F27" s="120" t="s">
         <v>47</v>
       </c>
-      <c r="G27" s="121"/>
-      <c r="H27" s="121"/>
-      <c r="I27" s="119" t="s">
+      <c r="G27" s="120"/>
+      <c r="H27" s="120"/>
+      <c r="I27" s="121" t="s">
         <v>48</v>
       </c>
-      <c r="J27" s="119"/>
-      <c r="K27" s="119"/>
-      <c r="L27" s="119" t="s">
+      <c r="J27" s="121"/>
+      <c r="K27" s="121"/>
+      <c r="L27" s="121" t="s">
         <v>127</v>
       </c>
-      <c r="M27" s="119"/>
-      <c r="N27" s="119"/>
+      <c r="M27" s="121"/>
+      <c r="N27" s="121"/>
     </row>
     <row r="28" spans="1:24" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="29" spans="1:24" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="1:24" s="18" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A30" s="120" t="s">
+      <c r="A30" s="119" t="s">
         <v>128</v>
       </c>
-      <c r="B30" s="120"/>
-      <c r="C30" s="120"/>
-      <c r="D30" s="120"/>
-      <c r="E30" s="120"/>
-      <c r="F30" s="120"/>
-      <c r="G30" s="120"/>
-      <c r="H30" s="120"/>
-      <c r="I30" s="120"/>
-      <c r="J30" s="120"/>
-      <c r="K30" s="120"/>
-      <c r="L30" s="120"/>
-      <c r="M30" s="120"/>
-      <c r="N30" s="120"/>
-      <c r="O30" s="120"/>
-      <c r="P30" s="120"/>
-      <c r="Q30" s="120"/>
+      <c r="B30" s="119"/>
+      <c r="C30" s="119"/>
+      <c r="D30" s="119"/>
+      <c r="E30" s="119"/>
+      <c r="F30" s="119"/>
+      <c r="G30" s="119"/>
+      <c r="H30" s="119"/>
+      <c r="I30" s="119"/>
+      <c r="J30" s="119"/>
+      <c r="K30" s="119"/>
+      <c r="L30" s="119"/>
+      <c r="M30" s="119"/>
+      <c r="N30" s="119"/>
+      <c r="O30" s="119"/>
+      <c r="P30" s="119"/>
+      <c r="Q30" s="119"/>
     </row>
     <row r="31" spans="1:24" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="37" t="s">
@@ -7615,26 +7615,26 @@
       <c r="E31" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="F31" s="125" t="s">
+      <c r="F31" s="122" t="s">
         <v>47</v>
       </c>
-      <c r="G31" s="126"/>
-      <c r="H31" s="127"/>
-      <c r="I31" s="125" t="s">
+      <c r="G31" s="123"/>
+      <c r="H31" s="124"/>
+      <c r="I31" s="122" t="s">
         <v>48</v>
       </c>
-      <c r="J31" s="126"/>
-      <c r="K31" s="127"/>
-      <c r="L31" s="119" t="s">
+      <c r="J31" s="123"/>
+      <c r="K31" s="124"/>
+      <c r="L31" s="121" t="s">
         <v>129</v>
       </c>
-      <c r="M31" s="119"/>
-      <c r="N31" s="119"/>
-      <c r="O31" s="119" t="s">
+      <c r="M31" s="121"/>
+      <c r="N31" s="121"/>
+      <c r="O31" s="121" t="s">
         <v>130</v>
       </c>
-      <c r="P31" s="119"/>
-      <c r="Q31" s="119"/>
+      <c r="P31" s="121"/>
+      <c r="Q31" s="121"/>
     </row>
     <row r="32" spans="1:24" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="20"/>
@@ -7669,14 +7669,14 @@
       <c r="R33"/>
     </row>
     <row r="34" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A34" s="120" t="s">
+      <c r="A34" s="119" t="s">
         <v>15</v>
       </c>
-      <c r="B34" s="120"/>
-      <c r="C34" s="120"/>
-      <c r="D34" s="120"/>
-      <c r="E34" s="120"/>
-      <c r="F34" s="120"/>
+      <c r="B34" s="119"/>
+      <c r="C34" s="119"/>
+      <c r="D34" s="119"/>
+      <c r="E34" s="119"/>
+      <c r="F34" s="119"/>
       <c r="G34" s="11"/>
       <c r="S34" s="10"/>
       <c r="T34" s="10"/>
@@ -7753,12 +7753,12 @@
       <c r="X37" s="10"/>
     </row>
     <row r="38" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A38" s="120" t="s">
+      <c r="A38" s="119" t="s">
         <v>19</v>
       </c>
-      <c r="B38" s="120"/>
-      <c r="C38" s="120"/>
-      <c r="D38" s="120"/>
+      <c r="B38" s="119"/>
+      <c r="C38" s="119"/>
+      <c r="D38" s="119"/>
       <c r="E38" s="11"/>
       <c r="F38" s="11"/>
       <c r="G38" s="11"/>
@@ -7824,15 +7824,15 @@
       <c r="G41" s="11"/>
     </row>
     <row r="42" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A42" s="122" t="s">
+      <c r="A42" s="125" t="s">
         <v>20</v>
       </c>
-      <c r="B42" s="123"/>
-      <c r="C42" s="123"/>
-      <c r="D42" s="123"/>
-      <c r="E42" s="123"/>
-      <c r="F42" s="123"/>
-      <c r="G42" s="124"/>
+      <c r="B42" s="126"/>
+      <c r="C42" s="126"/>
+      <c r="D42" s="126"/>
+      <c r="E42" s="126"/>
+      <c r="F42" s="126"/>
+      <c r="G42" s="127"/>
     </row>
     <row r="43" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A43" s="68" t="s">
@@ -7847,11 +7847,11 @@
       <c r="D43" s="68" t="s">
         <v>16</v>
       </c>
-      <c r="E43" s="119" t="s">
+      <c r="E43" s="121" t="s">
         <v>21</v>
       </c>
-      <c r="F43" s="119"/>
-      <c r="G43" s="119"/>
+      <c r="F43" s="121"/>
+      <c r="G43" s="121"/>
     </row>
     <row r="44" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="47"/>
@@ -8022,21 +8022,6 @@
     <row r="65" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="A8:N8"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="A5:K5"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="A12:K12"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="I13:K13"/>
-    <mergeCell ref="A18:K18"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="I19:K19"/>
     <mergeCell ref="E43:G43"/>
     <mergeCell ref="A22:K22"/>
     <mergeCell ref="F23:H23"/>
@@ -8053,6 +8038,21 @@
     <mergeCell ref="I31:K31"/>
     <mergeCell ref="L31:N31"/>
     <mergeCell ref="O31:Q31"/>
+    <mergeCell ref="A12:K12"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="I13:K13"/>
+    <mergeCell ref="A18:K18"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="A8:N8"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="A5:K5"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="I6:K6"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B21" xr:uid="{00000000-0002-0000-0100-000001000000}">
@@ -8171,7 +8171,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F55610B-D925-4735-AE3D-EBBD0AD81ACC}">
   <dimension ref="A1:AA21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
@@ -8195,58 +8195,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="142" t="s">
+      <c r="A1" s="134" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="143"/>
-      <c r="C1" s="143"/>
-      <c r="D1" s="143"/>
-      <c r="E1" s="143"/>
-      <c r="F1" s="143"/>
-      <c r="G1" s="143"/>
-      <c r="H1" s="143"/>
-      <c r="I1" s="143"/>
-      <c r="J1" s="143"/>
-      <c r="K1" s="143"/>
-      <c r="L1" s="143"/>
-      <c r="M1" s="143"/>
-      <c r="N1" s="143"/>
-      <c r="O1" s="143"/>
-      <c r="P1" s="143"/>
-      <c r="Q1" s="143"/>
-      <c r="R1" s="143"/>
-      <c r="S1" s="143"/>
+      <c r="B1" s="135"/>
+      <c r="C1" s="135"/>
+      <c r="D1" s="135"/>
+      <c r="E1" s="135"/>
+      <c r="F1" s="135"/>
+      <c r="G1" s="135"/>
+      <c r="H1" s="135"/>
+      <c r="I1" s="135"/>
+      <c r="J1" s="135"/>
+      <c r="K1" s="135"/>
+      <c r="L1" s="135"/>
+      <c r="M1" s="135"/>
+      <c r="N1" s="135"/>
+      <c r="O1" s="135"/>
+      <c r="P1" s="135"/>
+      <c r="Q1" s="135"/>
+      <c r="R1" s="135"/>
+      <c r="S1" s="135"/>
     </row>
     <row r="2" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="120"/>
-      <c r="B2" s="120"/>
-      <c r="C2" s="120"/>
-      <c r="D2" s="120"/>
-      <c r="E2" s="120"/>
-      <c r="F2" s="120"/>
-      <c r="G2" s="120"/>
-      <c r="H2" s="120"/>
-      <c r="I2" s="120"/>
-      <c r="J2" s="120"/>
-      <c r="K2" s="120"/>
-      <c r="L2" s="120"/>
-      <c r="M2" s="120"/>
-      <c r="N2" s="145" t="s">
+      <c r="A2" s="119"/>
+      <c r="B2" s="119"/>
+      <c r="C2" s="119"/>
+      <c r="D2" s="119"/>
+      <c r="E2" s="119"/>
+      <c r="F2" s="119"/>
+      <c r="G2" s="119"/>
+      <c r="H2" s="119"/>
+      <c r="I2" s="119"/>
+      <c r="J2" s="119"/>
+      <c r="K2" s="119"/>
+      <c r="L2" s="119"/>
+      <c r="M2" s="119"/>
+      <c r="N2" s="136" t="s">
         <v>115</v>
       </c>
-      <c r="O2" s="146"/>
-      <c r="P2" s="146"/>
-      <c r="Q2" s="146"/>
-      <c r="R2" s="146"/>
-      <c r="S2" s="147"/>
-      <c r="V2" s="133" t="s">
+      <c r="O2" s="137"/>
+      <c r="P2" s="137"/>
+      <c r="Q2" s="137"/>
+      <c r="R2" s="137"/>
+      <c r="S2" s="138"/>
+      <c r="V2" s="143" t="s">
         <v>123</v>
       </c>
-      <c r="W2" s="133"/>
-      <c r="X2" s="133"/>
-      <c r="Y2" s="133"/>
-      <c r="Z2" s="133"/>
-      <c r="AA2" s="133"/>
+      <c r="W2" s="143"/>
+      <c r="X2" s="143"/>
+      <c r="Y2" s="143"/>
+      <c r="Z2" s="143"/>
+      <c r="AA2" s="143"/>
     </row>
     <row r="3" spans="1:27" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="37" t="s">
@@ -8264,16 +8264,16 @@
       <c r="E3" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="134" t="s">
+      <c r="F3" s="144" t="s">
         <v>47</v>
       </c>
-      <c r="G3" s="135"/>
-      <c r="H3" s="136"/>
-      <c r="I3" s="138" t="s">
+      <c r="G3" s="145"/>
+      <c r="H3" s="146"/>
+      <c r="I3" s="148" t="s">
         <v>48</v>
       </c>
-      <c r="J3" s="139"/>
-      <c r="K3" s="140"/>
+      <c r="J3" s="149"/>
+      <c r="K3" s="150"/>
       <c r="L3" s="65" t="s">
         <v>249</v>
       </c>
@@ -8292,16 +8292,16 @@
       <c r="Q3" s="40" t="s">
         <v>120</v>
       </c>
-      <c r="R3" s="137" t="s">
+      <c r="R3" s="147" t="s">
         <v>122</v>
       </c>
-      <c r="S3" s="137"/>
-      <c r="V3" s="133"/>
-      <c r="W3" s="133"/>
-      <c r="X3" s="133"/>
-      <c r="Y3" s="133"/>
-      <c r="Z3" s="133"/>
-      <c r="AA3" s="133"/>
+      <c r="S3" s="147"/>
+      <c r="V3" s="143"/>
+      <c r="W3" s="143"/>
+      <c r="X3" s="143"/>
+      <c r="Y3" s="143"/>
+      <c r="Z3" s="143"/>
+      <c r="AA3" s="143"/>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B4" s="47" t="s">
@@ -8332,21 +8332,23 @@
       <c r="K4" s="47">
         <v>0</v>
       </c>
-      <c r="L4" s="47"/>
+      <c r="L4" s="47">
+        <v>500</v>
+      </c>
       <c r="M4" s="18">
-        <v>80</v>
+        <v>800</v>
       </c>
       <c r="N4" s="41"/>
       <c r="O4" s="18"/>
       <c r="P4" s="18"/>
       <c r="Q4" s="18"/>
       <c r="R4" s="18"/>
-      <c r="V4" s="133"/>
-      <c r="W4" s="133"/>
-      <c r="X4" s="133"/>
-      <c r="Y4" s="133"/>
-      <c r="Z4" s="133"/>
-      <c r="AA4" s="133"/>
+      <c r="V4" s="143"/>
+      <c r="W4" s="143"/>
+      <c r="X4" s="143"/>
+      <c r="Y4" s="143"/>
+      <c r="Z4" s="143"/>
+      <c r="AA4" s="143"/>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="47"/>
@@ -8378,9 +8380,11 @@
       <c r="K5" s="47">
         <v>0</v>
       </c>
-      <c r="L5" s="47"/>
+      <c r="L5" s="47">
+        <v>500</v>
+      </c>
       <c r="M5" s="18">
-        <v>80</v>
+        <v>800</v>
       </c>
       <c r="N5" s="47"/>
       <c r="O5" s="47"/>
@@ -8388,76 +8392,76 @@
       <c r="Q5" s="47"/>
       <c r="R5" s="47"/>
       <c r="S5" s="47"/>
-      <c r="V5" s="133"/>
-      <c r="W5" s="133"/>
-      <c r="X5" s="133"/>
-      <c r="Y5" s="133"/>
-      <c r="Z5" s="133"/>
-      <c r="AA5" s="133"/>
+      <c r="V5" s="143"/>
+      <c r="W5" s="143"/>
+      <c r="X5" s="143"/>
+      <c r="Y5" s="143"/>
+      <c r="Z5" s="143"/>
+      <c r="AA5" s="143"/>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="V6" s="133"/>
-      <c r="W6" s="133"/>
-      <c r="X6" s="133"/>
-      <c r="Y6" s="133"/>
-      <c r="Z6" s="133"/>
-      <c r="AA6" s="133"/>
+      <c r="V6" s="143"/>
+      <c r="W6" s="143"/>
+      <c r="X6" s="143"/>
+      <c r="Y6" s="143"/>
+      <c r="Z6" s="143"/>
+      <c r="AA6" s="143"/>
     </row>
     <row r="7" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="142" t="s">
+      <c r="A7" s="134" t="s">
         <v>73</v>
       </c>
-      <c r="B7" s="143"/>
-      <c r="C7" s="143"/>
-      <c r="D7" s="143"/>
-      <c r="E7" s="143"/>
-      <c r="F7" s="143"/>
-      <c r="G7" s="143"/>
-      <c r="H7" s="143"/>
-      <c r="I7" s="143"/>
-      <c r="J7" s="143"/>
-      <c r="K7" s="143"/>
-      <c r="L7" s="143"/>
-      <c r="M7" s="143"/>
-      <c r="N7" s="143"/>
-      <c r="O7" s="143"/>
-      <c r="P7" s="143"/>
-      <c r="Q7" s="143"/>
-      <c r="R7" s="143"/>
-      <c r="V7" s="133"/>
-      <c r="W7" s="133"/>
-      <c r="X7" s="133"/>
-      <c r="Y7" s="133"/>
-      <c r="Z7" s="133"/>
-      <c r="AA7" s="133"/>
+      <c r="B7" s="135"/>
+      <c r="C7" s="135"/>
+      <c r="D7" s="135"/>
+      <c r="E7" s="135"/>
+      <c r="F7" s="135"/>
+      <c r="G7" s="135"/>
+      <c r="H7" s="135"/>
+      <c r="I7" s="135"/>
+      <c r="J7" s="135"/>
+      <c r="K7" s="135"/>
+      <c r="L7" s="135"/>
+      <c r="M7" s="135"/>
+      <c r="N7" s="135"/>
+      <c r="O7" s="135"/>
+      <c r="P7" s="135"/>
+      <c r="Q7" s="135"/>
+      <c r="R7" s="135"/>
+      <c r="V7" s="143"/>
+      <c r="W7" s="143"/>
+      <c r="X7" s="143"/>
+      <c r="Y7" s="143"/>
+      <c r="Z7" s="143"/>
+      <c r="AA7" s="143"/>
     </row>
     <row r="8" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="120"/>
-      <c r="B8" s="120"/>
-      <c r="C8" s="120"/>
-      <c r="D8" s="120"/>
-      <c r="E8" s="120"/>
-      <c r="F8" s="120"/>
-      <c r="G8" s="120"/>
-      <c r="H8" s="120"/>
-      <c r="I8" s="120"/>
-      <c r="J8" s="120"/>
-      <c r="K8" s="120"/>
-      <c r="L8" s="120"/>
-      <c r="M8" s="120"/>
-      <c r="N8" s="141" t="s">
+      <c r="A8" s="119"/>
+      <c r="B8" s="119"/>
+      <c r="C8" s="119"/>
+      <c r="D8" s="119"/>
+      <c r="E8" s="119"/>
+      <c r="F8" s="119"/>
+      <c r="G8" s="119"/>
+      <c r="H8" s="119"/>
+      <c r="I8" s="119"/>
+      <c r="J8" s="119"/>
+      <c r="K8" s="119"/>
+      <c r="L8" s="119"/>
+      <c r="M8" s="119"/>
+      <c r="N8" s="151" t="s">
         <v>119</v>
       </c>
-      <c r="O8" s="141"/>
-      <c r="P8" s="141"/>
-      <c r="Q8" s="141"/>
-      <c r="R8" s="141"/>
-      <c r="V8" s="133"/>
-      <c r="W8" s="133"/>
-      <c r="X8" s="133"/>
-      <c r="Y8" s="133"/>
-      <c r="Z8" s="133"/>
-      <c r="AA8" s="133"/>
+      <c r="O8" s="151"/>
+      <c r="P8" s="151"/>
+      <c r="Q8" s="151"/>
+      <c r="R8" s="151"/>
+      <c r="V8" s="143"/>
+      <c r="W8" s="143"/>
+      <c r="X8" s="143"/>
+      <c r="Y8" s="143"/>
+      <c r="Z8" s="143"/>
+      <c r="AA8" s="143"/>
     </row>
     <row r="9" spans="1:27" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="37" t="s">
@@ -8475,16 +8479,16 @@
       <c r="E9" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="134" t="s">
+      <c r="F9" s="144" t="s">
         <v>47</v>
       </c>
-      <c r="G9" s="135"/>
-      <c r="H9" s="136"/>
-      <c r="I9" s="138" t="s">
+      <c r="G9" s="145"/>
+      <c r="H9" s="146"/>
+      <c r="I9" s="148" t="s">
         <v>48</v>
       </c>
-      <c r="J9" s="139"/>
-      <c r="K9" s="140"/>
+      <c r="J9" s="149"/>
+      <c r="K9" s="150"/>
       <c r="L9" s="40" t="s">
         <v>114</v>
       </c>
@@ -8500,16 +8504,16 @@
       <c r="P9" s="43" t="s">
         <v>120</v>
       </c>
-      <c r="Q9" s="134" t="s">
+      <c r="Q9" s="144" t="s">
         <v>121</v>
       </c>
-      <c r="R9" s="136"/>
-      <c r="V9" s="133"/>
-      <c r="W9" s="133"/>
-      <c r="X9" s="133"/>
-      <c r="Y9" s="133"/>
-      <c r="Z9" s="133"/>
-      <c r="AA9" s="133"/>
+      <c r="R9" s="146"/>
+      <c r="V9" s="143"/>
+      <c r="W9" s="143"/>
+      <c r="X9" s="143"/>
+      <c r="Y9" s="143"/>
+      <c r="Z9" s="143"/>
+      <c r="AA9" s="143"/>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="38"/>
@@ -8545,12 +8549,12 @@
         <v>40</v>
       </c>
       <c r="M10" s="26"/>
-      <c r="V10" s="133"/>
-      <c r="W10" s="133"/>
-      <c r="X10" s="133"/>
-      <c r="Y10" s="133"/>
-      <c r="Z10" s="133"/>
-      <c r="AA10" s="133"/>
+      <c r="V10" s="143"/>
+      <c r="W10" s="143"/>
+      <c r="X10" s="143"/>
+      <c r="Y10" s="143"/>
+      <c r="Z10" s="143"/>
+      <c r="AA10" s="143"/>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="38"/>
@@ -8585,51 +8589,51 @@
       <c r="L11" s="47">
         <v>40</v>
       </c>
-      <c r="V11" s="133"/>
-      <c r="W11" s="133"/>
-      <c r="X11" s="133"/>
-      <c r="Y11" s="133"/>
-      <c r="Z11" s="133"/>
-      <c r="AA11" s="133"/>
+      <c r="V11" s="143"/>
+      <c r="W11" s="143"/>
+      <c r="X11" s="143"/>
+      <c r="Y11" s="143"/>
+      <c r="Z11" s="143"/>
+      <c r="AA11" s="143"/>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="Q12" s="47"/>
-      <c r="V12" s="133"/>
-      <c r="W12" s="133"/>
-      <c r="X12" s="133"/>
-      <c r="Y12" s="133"/>
-      <c r="Z12" s="133"/>
-      <c r="AA12" s="133"/>
+      <c r="V12" s="143"/>
+      <c r="W12" s="143"/>
+      <c r="X12" s="143"/>
+      <c r="Y12" s="143"/>
+      <c r="Z12" s="143"/>
+      <c r="AA12" s="143"/>
     </row>
     <row r="13" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A13" s="122" t="s">
+      <c r="A13" s="125" t="s">
         <v>78</v>
       </c>
-      <c r="B13" s="123"/>
-      <c r="C13" s="123"/>
-      <c r="D13" s="123"/>
-      <c r="E13" s="123"/>
-      <c r="F13" s="123"/>
-      <c r="G13" s="123"/>
-      <c r="H13" s="123"/>
-      <c r="I13" s="123"/>
-      <c r="J13" s="123"/>
-      <c r="K13" s="123"/>
-      <c r="L13" s="123"/>
-      <c r="M13" s="123"/>
-      <c r="N13" s="123"/>
-      <c r="O13" s="123"/>
-      <c r="P13" s="123"/>
+      <c r="B13" s="126"/>
+      <c r="C13" s="126"/>
+      <c r="D13" s="126"/>
+      <c r="E13" s="126"/>
+      <c r="F13" s="126"/>
+      <c r="G13" s="126"/>
+      <c r="H13" s="126"/>
+      <c r="I13" s="126"/>
+      <c r="J13" s="126"/>
+      <c r="K13" s="126"/>
+      <c r="L13" s="126"/>
+      <c r="M13" s="126"/>
+      <c r="N13" s="126"/>
+      <c r="O13" s="126"/>
+      <c r="P13" s="126"/>
       <c r="Q13" s="47"/>
       <c r="R13" s="35"/>
       <c r="S13" s="35"/>
       <c r="T13" s="35"/>
-      <c r="V13" s="133"/>
-      <c r="W13" s="133"/>
-      <c r="X13" s="133"/>
-      <c r="Y13" s="133"/>
-      <c r="Z13" s="133"/>
-      <c r="AA13" s="133"/>
+      <c r="V13" s="143"/>
+      <c r="W13" s="143"/>
+      <c r="X13" s="143"/>
+      <c r="Y13" s="143"/>
+      <c r="Z13" s="143"/>
+      <c r="AA13" s="143"/>
     </row>
     <row r="14" spans="1:27" s="35" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="34" t="s">
@@ -8647,24 +8651,24 @@
       <c r="E14" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="F14" s="144" t="s">
+      <c r="F14" s="133" t="s">
         <v>83</v>
       </c>
-      <c r="G14" s="144"/>
-      <c r="H14" s="144"/>
+      <c r="G14" s="133"/>
+      <c r="H14" s="133"/>
       <c r="I14" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="J14" s="149" t="s">
+      <c r="J14" s="140" t="s">
         <v>11</v>
       </c>
-      <c r="K14" s="150"/>
-      <c r="L14" s="151"/>
-      <c r="M14" s="148" t="s">
+      <c r="K14" s="141"/>
+      <c r="L14" s="142"/>
+      <c r="M14" s="139" t="s">
         <v>77</v>
       </c>
-      <c r="N14" s="148"/>
-      <c r="O14" s="148"/>
+      <c r="N14" s="139"/>
+      <c r="O14" s="139"/>
       <c r="P14" s="36" t="s">
         <v>79</v>
       </c>
@@ -8715,20 +8719,20 @@
       <c r="T16" s="38"/>
     </row>
     <row r="17" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A17" s="120" t="s">
+      <c r="A17" s="119" t="s">
         <v>151</v>
       </c>
-      <c r="B17" s="120"/>
-      <c r="C17" s="120"/>
-      <c r="D17" s="120"/>
-      <c r="E17" s="120"/>
-      <c r="F17" s="120"/>
-      <c r="G17" s="120"/>
-      <c r="H17" s="120"/>
-      <c r="I17" s="120"/>
-      <c r="J17" s="120"/>
-      <c r="K17" s="120"/>
-      <c r="L17" s="120"/>
+      <c r="B17" s="119"/>
+      <c r="C17" s="119"/>
+      <c r="D17" s="119"/>
+      <c r="E17" s="119"/>
+      <c r="F17" s="119"/>
+      <c r="G17" s="119"/>
+      <c r="H17" s="119"/>
+      <c r="I17" s="119"/>
+      <c r="J17" s="119"/>
+      <c r="K17" s="119"/>
+      <c r="L17" s="119"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="45" t="s">
@@ -8746,16 +8750,16 @@
       <c r="E18" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="F18" s="84" t="s">
+      <c r="F18" s="72" t="s">
         <v>21</v>
       </c>
-      <c r="G18" s="84"/>
-      <c r="H18" s="84"/>
-      <c r="I18" s="82" t="s">
+      <c r="G18" s="72"/>
+      <c r="H18" s="72"/>
+      <c r="I18" s="94" t="s">
         <v>160</v>
       </c>
-      <c r="J18" s="115"/>
-      <c r="K18" s="83"/>
+      <c r="J18" s="118"/>
+      <c r="K18" s="95"/>
       <c r="L18" s="33" t="s">
         <v>161</v>
       </c>
@@ -8807,15 +8811,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="I18:K18"/>
-    <mergeCell ref="A17:L17"/>
-    <mergeCell ref="A1:S1"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="N2:S2"/>
-    <mergeCell ref="M14:O14"/>
-    <mergeCell ref="J14:L14"/>
     <mergeCell ref="V2:AA13"/>
     <mergeCell ref="F3:H3"/>
     <mergeCell ref="R3:S3"/>
@@ -8827,6 +8822,15 @@
     <mergeCell ref="Q9:R9"/>
     <mergeCell ref="N8:R8"/>
     <mergeCell ref="A7:R7"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="A17:L17"/>
+    <mergeCell ref="A1:S1"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="N2:S2"/>
+    <mergeCell ref="M14:O14"/>
+    <mergeCell ref="J14:L14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8849,21 +8853,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="120" t="s">
+      <c r="A1" s="119" t="s">
         <v>236</v>
       </c>
-      <c r="B1" s="120"/>
-      <c r="C1" s="120"/>
-      <c r="F1" s="109" t="s">
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="F1" s="75" t="s">
         <v>157</v>
       </c>
-      <c r="G1" s="111"/>
-      <c r="I1" s="109" t="s">
+      <c r="G1" s="77"/>
+      <c r="I1" s="75" t="s">
         <v>240</v>
       </c>
-      <c r="J1" s="110"/>
-      <c r="K1" s="110"/>
-      <c r="L1" s="111"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
+      <c r="L1" s="77"/>
     </row>
     <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="60" t="s">
@@ -8881,12 +8885,12 @@
       <c r="G2" s="60" t="s">
         <v>134</v>
       </c>
-      <c r="I2" s="133" t="s">
+      <c r="I2" s="143" t="s">
         <v>239</v>
       </c>
-      <c r="J2" s="133"/>
-      <c r="K2" s="133"/>
-      <c r="L2" s="133"/>
+      <c r="J2" s="143"/>
+      <c r="K2" s="143"/>
+      <c r="L2" s="143"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="60"/>
@@ -8898,10 +8902,10 @@
       <c r="G3" s="61" t="s">
         <v>166</v>
       </c>
-      <c r="I3" s="133"/>
-      <c r="J3" s="133"/>
-      <c r="K3" s="133"/>
-      <c r="L3" s="133"/>
+      <c r="I3" s="143"/>
+      <c r="J3" s="143"/>
+      <c r="K3" s="143"/>
+      <c r="L3" s="143"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="60"/>
@@ -8913,10 +8917,10 @@
       <c r="G4" s="61" t="s">
         <v>167</v>
       </c>
-      <c r="I4" s="133"/>
-      <c r="J4" s="133"/>
-      <c r="K4" s="133"/>
-      <c r="L4" s="133"/>
+      <c r="I4" s="143"/>
+      <c r="J4" s="143"/>
+      <c r="K4" s="143"/>
+      <c r="L4" s="143"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="60"/>
@@ -8928,10 +8932,10 @@
       <c r="G5" s="61" t="s">
         <v>170</v>
       </c>
-      <c r="I5" s="133"/>
-      <c r="J5" s="133"/>
-      <c r="K5" s="133"/>
-      <c r="L5" s="133"/>
+      <c r="I5" s="143"/>
+      <c r="J5" s="143"/>
+      <c r="K5" s="143"/>
+      <c r="L5" s="143"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="60"/>
@@ -8943,10 +8947,10 @@
       <c r="G6" s="61" t="s">
         <v>171</v>
       </c>
-      <c r="I6" s="133"/>
-      <c r="J6" s="133"/>
-      <c r="K6" s="133"/>
-      <c r="L6" s="133"/>
+      <c r="I6" s="143"/>
+      <c r="J6" s="143"/>
+      <c r="K6" s="143"/>
+      <c r="L6" s="143"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="60"/>

</xml_diff>